<commit_message>
Made second refactor (for excel)
</commit_message>
<xml_diff>
--- a/BitcoinPriceTracker/Data/prices.xlsx
+++ b/BitcoinPriceTracker/Data/prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8319DB-5AC7-497C-8308-A705544EB2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCDAD51-E636-4817-84BB-7BAE92857F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30945" yWindow="2040" windowWidth="17910" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>Old Prices</t>
   </si>
   <si>
-    <t>46662.41 </t>
-  </si>
-  <si>
     <t>46155.04 </t>
+  </si>
+  <si>
+    <t>46131.60 </t>
   </si>
 </sst>
 </file>
@@ -435,13 +435,13 @@
         <v>0</v>
       </c>
       <c r="B2">
+        <v>46071.03</v>
+      </c>
+      <c r="C2" s="1">
+        <v>40562.879999999997</v>
+      </c>
+      <c r="D2">
         <v>46080.68</v>
-      </c>
-      <c r="C2" s="1">
-        <v>40571.379999999997</v>
-      </c>
-      <c r="D2">
-        <v>46821.07</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -449,13 +449,13 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>46066.400000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40558.81</v>
+      </c>
+      <c r="D3">
         <v>46071.19</v>
-      </c>
-      <c r="C3" s="1">
-        <v>40563.019999999997</v>
-      </c>
-      <c r="D3">
-        <v>46874.65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -463,13 +463,13 @@
         <v>2</v>
       </c>
       <c r="B4">
+        <v>46094.14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>40583.230000000003</v>
+      </c>
+      <c r="D4">
         <v>46087.23</v>
-      </c>
-      <c r="C4" s="1">
-        <v>40577.14</v>
-      </c>
-      <c r="D4">
-        <v>46827.42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -477,13 +477,13 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <v>46145.919999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40628.82</v>
+      </c>
+      <c r="D5">
         <v>46170.09</v>
-      </c>
-      <c r="C5" s="1">
-        <v>40650.1</v>
-      </c>
-      <c r="D5">
-        <v>46534.879999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>40636.85</v>
+        <v>40616.21</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
removed try catch from ReadOldPrices and changed browser interaction
</commit_message>
<xml_diff>
--- a/BitcoinPriceTracker/Data/prices.xlsx
+++ b/BitcoinPriceTracker/Data/prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Gabor\Desktop\UNI\3rd YEAR\RPA\RPAProject\BitcoinPriceTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCDAD51-E636-4817-84BB-7BAE92857F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7ACA10-A25F-4D83-9E32-816BC94BB265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30945" yWindow="2040" windowWidth="17910" windowHeight="11325" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>Old Prices</t>
   </si>
   <si>
-    <t>46155.04 </t>
-  </si>
-  <si>
     <t>46131.60 </t>
+  </si>
+  <si>
+    <t>46276.50 </t>
   </si>
 </sst>
 </file>
@@ -435,13 +435,13 @@
         <v>0</v>
       </c>
       <c r="B2">
+        <v>46217.93</v>
+      </c>
+      <c r="C2" s="1">
+        <v>40692.22</v>
+      </c>
+      <c r="D2">
         <v>46071.03</v>
-      </c>
-      <c r="C2" s="1">
-        <v>40562.879999999997</v>
-      </c>
-      <c r="D2">
-        <v>46080.68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -449,13 +449,13 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>46215.1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40689.730000000003</v>
+      </c>
+      <c r="D3">
         <v>46066.400000000001</v>
-      </c>
-      <c r="C3" s="1">
-        <v>40558.81</v>
-      </c>
-      <c r="D3">
-        <v>46071.19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -463,13 +463,13 @@
         <v>2</v>
       </c>
       <c r="B4">
+        <v>46192.2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>40669.56</v>
+      </c>
+      <c r="D4">
         <v>46094.14</v>
-      </c>
-      <c r="C4" s="1">
-        <v>40583.230000000003</v>
-      </c>
-      <c r="D4">
-        <v>46087.23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -477,13 +477,13 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <v>46197.55</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40674.28</v>
+      </c>
+      <c r="D5">
         <v>46145.919999999998</v>
-      </c>
-      <c r="C5" s="1">
-        <v>40628.82</v>
-      </c>
-      <c r="D5">
-        <v>46170.09</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>40616.21</v>
+        <v>40743.79</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>

</xml_diff>